<commit_message>
Updated the planning worksheet with new sheet titled Sample Plan that lays out our decided on plan.  Created file in project plan called dive logs and stored the 2017 and 2018 dive logs in there already sorted for easy access.  Updated the readme before these most recent changes so it needs to be updated again.
</commit_message>
<xml_diff>
--- a/Project_Plan/Analysis_Time_Worksheet_11Feb2019JKB.xlsx
+++ b/Project_Plan/Analysis_Time_Worksheet_11Feb2019JKB.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julia_2013MacBookAir/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FB46AF-5B3E-4829-AC48-049DFE7ED8FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,12 +25,15 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>Sound Analysis Time</t>
   </si>
@@ -188,19 +185,88 @@
     <t>Days with divers in water - June 2018</t>
   </si>
   <si>
-    <t>11, 23</t>
-  </si>
-  <si>
-    <t>17, 25</t>
-  </si>
-  <si>
     <t xml:space="preserve">+ extra one(s) you've already processed?? </t>
+  </si>
+  <si>
+    <t>17, 19, 23, 30</t>
+  </si>
+  <si>
+    <t>15, 17, 21, 28, 2</t>
+  </si>
+  <si>
+    <t>14, 19, 22, 1</t>
+  </si>
+  <si>
+    <t>15, 18, 21, 29</t>
+  </si>
+  <si>
+    <t>14, 18, 21, 29, 1</t>
+  </si>
+  <si>
+    <t>7, 9, 20</t>
+  </si>
+  <si>
+    <t>10, 11, 23</t>
+  </si>
+  <si>
+    <t>14, 17, 18, 25</t>
+  </si>
+  <si>
+    <t>6, 11, 23, 24</t>
+  </si>
+  <si>
+    <t>16, 20, 22, 28</t>
+  </si>
+  <si>
+    <t>Sampling Scheme</t>
+  </si>
+  <si>
+    <t>To lay out the sampling method that I am using for my acoustic analyses</t>
+  </si>
+  <si>
+    <t>Number of recordings in 2017</t>
+  </si>
+  <si>
+    <t>Number of recordings in 2018</t>
+  </si>
+  <si>
+    <t>Deployment ranges within each site in each year</t>
+  </si>
+  <si>
+    <t>Dates with divers in the water at each site during hydrophone deployment</t>
+  </si>
+  <si>
+    <t>2017 Site</t>
+  </si>
+  <si>
+    <t>2018 Site</t>
+  </si>
+  <si>
+    <t>Sampling Dates (another Sampling option)</t>
+  </si>
+  <si>
+    <t>Every other day (with adjustments around initial days with divers)</t>
+  </si>
+  <si>
+    <t>Days already processed 2018</t>
+  </si>
+  <si>
+    <t>Dates already analyzed (only 2018 was analyzed)</t>
+  </si>
+  <si>
+    <t>15, 16</t>
+  </si>
+  <si>
+    <t>16, 17</t>
+  </si>
+  <si>
+    <t>18, 19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -257,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,8 +426,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -804,11 +876,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -909,18 +1142,169 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -960,139 +1344,201 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="2" fillId="7" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="49" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="50" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1379,30 +1825,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32:L36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="9.1640625" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>26</v>
       </c>
@@ -1413,7 +1860,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>28</v>
       </c>
@@ -1424,108 +1871,112 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-    </row>
-    <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+    </row>
+    <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="136"/>
       <c r="S4" s="10"/>
-    </row>
-    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="82"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="136"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="136"/>
+      <c r="R5" s="136"/>
       <c r="S5" s="10"/>
-    </row>
-    <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="136"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="136"/>
+      <c r="R6" s="136"/>
       <c r="S6" s="10"/>
-    </row>
-    <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="82"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="136"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="136"/>
+      <c r="K7" s="136"/>
+      <c r="L7" s="136"/>
+      <c r="M7" s="136"/>
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="136"/>
+      <c r="R7" s="136"/>
       <c r="S7" s="10"/>
-    </row>
-    <row r="8" spans="1:20" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="74" t="s">
         <v>32</v>
       </c>
@@ -1543,23 +1994,23 @@
       <c r="G8" s="65"/>
       <c r="H8" s="65"/>
       <c r="I8" s="65"/>
-      <c r="J8" s="106" t="s">
+      <c r="J8" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="92" t="s">
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="94"/>
+      <c r="O8" s="144"/>
+      <c r="P8" s="144"/>
+      <c r="Q8" s="145"/>
       <c r="R8" s="66"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
         <v>19</v>
       </c>
@@ -1575,23 +2026,23 @@
       <c r="E9" s="35"/>
       <c r="F9" s="55"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="115" t="s">
+      <c r="H9" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="115"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="97"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="146"/>
+      <c r="O9" s="147"/>
+      <c r="P9" s="147"/>
+      <c r="Q9" s="148"/>
       <c r="R9" s="35"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="80" t="s">
         <v>1</v>
       </c>
@@ -1623,10 +2074,10 @@
       <c r="K10" s="13">
         <v>40</v>
       </c>
-      <c r="L10" s="110" t="s">
+      <c r="L10" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="111"/>
+      <c r="M10" s="118"/>
       <c r="N10" s="47" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +2094,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="80" t="s">
         <v>37</v>
       </c>
@@ -1678,10 +2129,10 @@
       <c r="K11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="112" t="s">
+      <c r="L11" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="113"/>
+      <c r="M11" s="120"/>
       <c r="N11" s="51">
         <v>2017</v>
       </c>
@@ -1698,7 +2149,7 @@
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="80" t="s">
         <v>40</v>
       </c>
@@ -1739,7 +2190,7 @@
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="80" t="s">
         <v>39</v>
       </c>
@@ -1758,10 +2209,10 @@
       <c r="E13" s="10"/>
       <c r="F13" s="38"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="116" t="s">
+      <c r="H13" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="116"/>
+      <c r="I13" s="123"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="39"/>
@@ -1782,7 +2233,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="80" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +2289,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
         <v>14</v>
       </c>
@@ -1870,10 +2321,10 @@
       <c r="K15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="112" t="s">
+      <c r="L15" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="114"/>
+      <c r="M15" s="121"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1882,7 +2333,7 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -1904,7 +2355,7 @@
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="67" t="s">
         <v>3</v>
@@ -1913,26 +2364,26 @@
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
-      <c r="G17" s="132" t="s">
+      <c r="G17" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="132"/>
-      <c r="I17" s="132"/>
-      <c r="J17" s="132"/>
-      <c r="K17" s="142"/>
-      <c r="L17" s="133" t="s">
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="M17" s="134"/>
-      <c r="N17" s="134"/>
-      <c r="O17" s="134"/>
-      <c r="P17" s="135"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="94"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="17">
         <v>32</v>
@@ -1949,89 +2400,103 @@
       <c r="F18" s="12">
         <v>40</v>
       </c>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="132"/>
-      <c r="J18" s="132"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="136"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="138"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="95"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="97"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
-      <c r="I19" s="132"/>
-      <c r="J19" s="132"/>
-      <c r="K19" s="142"/>
-      <c r="L19" s="139"/>
-      <c r="M19" s="140"/>
-      <c r="N19" s="140"/>
-      <c r="O19" s="140"/>
-      <c r="P19" s="141"/>
+        <v>57</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="99"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="99"/>
+      <c r="P19" s="100"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="132"/>
-      <c r="H20" s="132"/>
-      <c r="I20" s="132"/>
-      <c r="J20" s="132"/>
-      <c r="K20" s="142"/>
-      <c r="L20" s="83" t="s">
+      <c r="B20" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="84"/>
-      <c r="N20" s="84"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="85"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
+      <c r="P20" s="103"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="132"/>
-      <c r="H21" s="132"/>
-      <c r="I21" s="132"/>
-      <c r="J21" s="132"/>
-      <c r="K21" s="142"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="105"/>
       <c r="L21" s="17">
         <v>32</v>
       </c>
@@ -2052,18 +2517,18 @@
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="132"/>
-      <c r="I22" s="132"/>
-      <c r="J22" s="132"/>
-      <c r="K22" s="142"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="105"/>
       <c r="L22" s="31">
         <v>12</v>
       </c>
@@ -2084,7 +2549,7 @@
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
@@ -2116,7 +2581,7 @@
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
     </row>
-    <row r="24" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
@@ -2148,7 +2613,7 @@
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
     </row>
-    <row r="25" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
@@ -2180,7 +2645,7 @@
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
     </row>
-    <row r="26" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
@@ -2212,7 +2677,7 @@
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
     </row>
-    <row r="27" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
@@ -2244,7 +2709,7 @@
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
     </row>
-    <row r="28" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
@@ -2276,7 +2741,7 @@
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
@@ -2288,27 +2753,27 @@
       <c r="I29" s="35"/>
       <c r="J29" s="35"/>
       <c r="K29" s="35"/>
-      <c r="L29" s="143" t="s">
-        <v>52</v>
-      </c>
-      <c r="M29" s="143" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="143" t="s">
-        <v>52</v>
-      </c>
-      <c r="O29" s="143" t="s">
-        <v>52</v>
-      </c>
-      <c r="P29" s="143" t="s">
-        <v>52</v>
+      <c r="L29" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="N29" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="P29" s="88" t="s">
+        <v>50</v>
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
     </row>
-    <row r="30" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
@@ -2320,19 +2785,19 @@
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
       <c r="K30" s="35"/>
-      <c r="L30" s="83" t="s">
+      <c r="L30" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="84"/>
-      <c r="N30" s="84"/>
-      <c r="O30" s="84"/>
-      <c r="P30" s="85"/>
+      <c r="M30" s="102"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="102"/>
+      <c r="P30" s="103"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
@@ -2364,7 +2829,7 @@
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
     </row>
-    <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
@@ -2396,7 +2861,7 @@
       <c r="S32" s="10"/>
       <c r="T32" s="10"/>
     </row>
-    <row r="33" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
@@ -2428,7 +2893,7 @@
       <c r="S33" s="10"/>
       <c r="T33" s="10"/>
     </row>
-    <row r="34" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
@@ -2460,7 +2925,7 @@
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
@@ -2492,7 +2957,7 @@
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
     </row>
-    <row r="36" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
@@ -2524,7 +2989,7 @@
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
     </row>
-    <row r="37" spans="1:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="35"/>
       <c r="C37" s="35"/>
@@ -2546,110 +3011,110 @@
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
     </row>
-    <row r="38" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="130" t="s">
+    <row r="38" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="117" t="s">
+      <c r="B38" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="123" t="s">
+      <c r="C38" s="125"/>
+      <c r="D38" s="125"/>
+      <c r="E38" s="125"/>
+      <c r="F38" s="126"/>
+      <c r="G38" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="124"/>
-      <c r="I38" s="124"/>
-      <c r="J38" s="124"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="86" t="s">
+      <c r="H38" s="131"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="131"/>
+      <c r="K38" s="132"/>
+      <c r="L38" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="M38" s="87"/>
-      <c r="N38" s="87"/>
-      <c r="O38" s="87"/>
-      <c r="P38" s="88"/>
+      <c r="M38" s="138"/>
+      <c r="N38" s="138"/>
+      <c r="O38" s="138"/>
+      <c r="P38" s="139"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="131"/>
-      <c r="B39" s="120"/>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-      <c r="F39" s="122"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="127"/>
-      <c r="I39" s="127"/>
-      <c r="J39" s="127"/>
-      <c r="K39" s="128"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="90"/>
-      <c r="O39" s="90"/>
-      <c r="P39" s="91"/>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="91"/>
+      <c r="B39" s="127"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="133"/>
+      <c r="H39" s="134"/>
+      <c r="I39" s="134"/>
+      <c r="J39" s="134"/>
+      <c r="K39" s="135"/>
+      <c r="L39" s="140"/>
+      <c r="M39" s="141"/>
+      <c r="N39" s="141"/>
+      <c r="O39" s="141"/>
+      <c r="P39" s="142"/>
       <c r="Q39" s="23"/>
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="14"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="131"/>
-      <c r="B40" s="120"/>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="121"/>
-      <c r="F40" s="122"/>
-      <c r="G40" s="126"/>
-      <c r="H40" s="127"/>
-      <c r="I40" s="127"/>
-      <c r="J40" s="127"/>
-      <c r="K40" s="128"/>
-      <c r="L40" s="89"/>
-      <c r="M40" s="90"/>
-      <c r="N40" s="90"/>
-      <c r="O40" s="90"/>
-      <c r="P40" s="91"/>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="91"/>
+      <c r="B40" s="127"/>
+      <c r="C40" s="128"/>
+      <c r="D40" s="128"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="133"/>
+      <c r="H40" s="134"/>
+      <c r="I40" s="134"/>
+      <c r="J40" s="134"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="140"/>
+      <c r="M40" s="141"/>
+      <c r="N40" s="141"/>
+      <c r="O40" s="141"/>
+      <c r="P40" s="142"/>
       <c r="Q40" s="23"/>
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
     </row>
-    <row r="41" spans="1:20" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
-      <c r="B41" s="83" t="s">
+      <c r="B41" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="83" t="s">
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="103"/>
+      <c r="G41" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="84"/>
-      <c r="K41" s="85"/>
-      <c r="L41" s="83" t="s">
+      <c r="H41" s="102"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="102"/>
+      <c r="K41" s="103"/>
+      <c r="L41" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M41" s="84"/>
-      <c r="N41" s="84"/>
-      <c r="O41" s="84"/>
-      <c r="P41" s="85"/>
+      <c r="M41" s="102"/>
+      <c r="N41" s="102"/>
+      <c r="O41" s="102"/>
+      <c r="P41" s="103"/>
       <c r="Q41" s="23"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
     </row>
-    <row r="42" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="99">
+    <row r="42" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="114">
         <v>42917</v>
       </c>
       <c r="B42" s="17">
@@ -2697,15 +3162,15 @@
       <c r="P42" s="12">
         <v>40</v>
       </c>
-      <c r="Q42" s="98" t="s">
+      <c r="Q42" s="149" t="s">
         <v>4</v>
       </c>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="100"/>
+    <row r="43" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="115"/>
       <c r="B43" s="57">
         <v>11</v>
       </c>
@@ -2751,13 +3216,13 @@
       <c r="P43" s="32">
         <v>11</v>
       </c>
-      <c r="Q43" s="98"/>
+      <c r="Q43" s="149"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="100"/>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="115"/>
       <c r="B44" s="57">
         <v>16</v>
       </c>
@@ -2803,13 +3268,13 @@
       <c r="P44" s="32">
         <v>13</v>
       </c>
-      <c r="Q44" s="98"/>
+      <c r="Q44" s="149"/>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="100"/>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="115"/>
       <c r="B45" s="57">
         <v>21</v>
       </c>
@@ -2855,13 +3320,13 @@
       <c r="P45" s="32">
         <v>15</v>
       </c>
-      <c r="Q45" s="98"/>
+      <c r="Q45" s="149"/>
       <c r="R45" s="10"/>
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="100"/>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="115"/>
       <c r="B46" s="57"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2897,13 +3362,13 @@
       <c r="P46" s="32">
         <v>17</v>
       </c>
-      <c r="Q46" s="98"/>
+      <c r="Q46" s="149"/>
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="100"/>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="115"/>
       <c r="B47" s="57"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2939,13 +3404,13 @@
       <c r="P47" s="32">
         <v>19</v>
       </c>
-      <c r="Q47" s="98"/>
+      <c r="Q47" s="149"/>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="100"/>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="115"/>
       <c r="B48" s="57"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -2971,13 +3436,13 @@
       <c r="P48" s="32">
         <v>21</v>
       </c>
-      <c r="Q48" s="98"/>
+      <c r="Q48" s="149"/>
       <c r="R48" s="10"/>
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
     </row>
-    <row r="49" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="100"/>
+    <row r="49" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="115"/>
       <c r="B49" s="57"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -3003,13 +3468,13 @@
       <c r="P49" s="32">
         <v>23</v>
       </c>
-      <c r="Q49" s="98"/>
+      <c r="Q49" s="149"/>
       <c r="R49" s="10"/>
       <c r="S49" s="16"/>
       <c r="T49" s="16"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="101"/>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="116"/>
       <c r="B50" s="57"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -3035,43 +3500,43 @@
       <c r="P50" s="32">
         <v>25</v>
       </c>
-      <c r="Q50" s="98"/>
+      <c r="Q50" s="149"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="99">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="114">
         <v>43252</v>
       </c>
-      <c r="B51" s="83" t="s">
+      <c r="B51" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="84"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="83" t="s">
+      <c r="C51" s="102"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="102"/>
+      <c r="F51" s="103"/>
+      <c r="G51" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="H51" s="84"/>
-      <c r="I51" s="84"/>
-      <c r="J51" s="84"/>
-      <c r="K51" s="85"/>
-      <c r="L51" s="83" t="s">
+      <c r="H51" s="102"/>
+      <c r="I51" s="102"/>
+      <c r="J51" s="102"/>
+      <c r="K51" s="103"/>
+      <c r="L51" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M51" s="84"/>
-      <c r="N51" s="84"/>
-      <c r="O51" s="84"/>
-      <c r="P51" s="85"/>
+      <c r="M51" s="102"/>
+      <c r="N51" s="102"/>
+      <c r="O51" s="102"/>
+      <c r="P51" s="103"/>
       <c r="Q51" s="58"/>
       <c r="R51" s="10"/>
       <c r="S51" s="10"/>
       <c r="T51" s="10"/>
     </row>
-    <row r="52" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="100"/>
+    <row r="52" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="115"/>
       <c r="B52" s="18">
         <v>32</v>
       </c>
@@ -3122,8 +3587,8 @@
       <c r="S52" s="10"/>
       <c r="T52" s="10"/>
     </row>
-    <row r="53" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="100"/>
+    <row r="53" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="115"/>
       <c r="B53" s="4">
         <v>18</v>
       </c>
@@ -3169,15 +3634,15 @@
       <c r="P53" s="73">
         <v>18</v>
       </c>
-      <c r="Q53" s="104" t="s">
+      <c r="Q53" s="108" t="s">
         <v>4</v>
       </c>
       <c r="R53" s="21"/>
       <c r="S53" s="10"/>
       <c r="T53" s="10"/>
     </row>
-    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="100"/>
+    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="115"/>
       <c r="B54" s="4">
         <v>23</v>
       </c>
@@ -3223,13 +3688,13 @@
       <c r="P54" s="32">
         <v>20</v>
       </c>
-      <c r="Q54" s="104"/>
+      <c r="Q54" s="108"/>
       <c r="R54" s="10"/>
       <c r="S54" s="10"/>
       <c r="T54" s="10"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="100"/>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="115"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -3265,13 +3730,13 @@
       <c r="P55" s="32">
         <v>22</v>
       </c>
-      <c r="Q55" s="104"/>
+      <c r="Q55" s="108"/>
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
       <c r="T55" s="10"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A56" s="100"/>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="115"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -3307,13 +3772,13 @@
       <c r="P56" s="32">
         <v>24</v>
       </c>
-      <c r="Q56" s="104"/>
+      <c r="Q56" s="108"/>
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
       <c r="T56" s="10"/>
     </row>
-    <row r="57" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="101"/>
+    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="116"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -3339,12 +3804,12 @@
       <c r="P57" s="34">
         <v>26</v>
       </c>
-      <c r="Q57" s="105"/>
+      <c r="Q57" s="109"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
       <c r="T57" s="10"/>
     </row>
-    <row r="58" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -3356,19 +3821,19 @@
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
-      <c r="L58" s="129" t="s">
+      <c r="L58" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="M58" s="129"/>
-      <c r="N58" s="129"/>
-      <c r="O58" s="129"/>
-      <c r="P58" s="129"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="89"/>
+      <c r="O58" s="89"/>
+      <c r="P58" s="89"/>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
       <c r="T58" s="10"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -3390,7 +3855,7 @@
       <c r="S59" s="10"/>
       <c r="T59" s="10"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -3412,7 +3877,7 @@
       <c r="S60" s="10"/>
       <c r="T60" s="10"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -3434,7 +3899,7 @@
       <c r="S61" s="10"/>
       <c r="T61" s="10"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -3456,7 +3921,7 @@
       <c r="S62" s="10"/>
       <c r="T62" s="10"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -3478,7 +3943,7 @@
       <c r="S63" s="10"/>
       <c r="T63" s="10"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -3500,7 +3965,7 @@
       <c r="S64" s="10"/>
       <c r="T64" s="10"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -3522,7 +3987,7 @@
       <c r="S65" s="10"/>
       <c r="T65" s="10"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -3544,7 +4009,7 @@
       <c r="S66" s="10"/>
       <c r="T66" s="10"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
@@ -3566,7 +4031,7 @@
       <c r="S67" s="10"/>
       <c r="T67" s="10"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -3588,7 +4053,7 @@
       <c r="S68" s="10"/>
       <c r="T68" s="10"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
@@ -3610,7 +4075,7 @@
       <c r="S69" s="10"/>
       <c r="T69" s="10"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -3632,7 +4097,7 @@
       <c r="S70" s="10"/>
       <c r="T70" s="10"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -3654,7 +4119,7 @@
       <c r="S71" s="10"/>
       <c r="T71" s="10"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -3676,7 +4141,7 @@
       <c r="S72" s="10"/>
       <c r="T72" s="10"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -3698,7 +4163,7 @@
       <c r="S73" s="10"/>
       <c r="T73" s="10"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -3720,7 +4185,7 @@
       <c r="S74" s="10"/>
       <c r="T74" s="10"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -3742,7 +4207,7 @@
       <c r="S75" s="10"/>
       <c r="T75" s="10"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -3764,7 +4229,7 @@
       <c r="S76" s="10"/>
       <c r="T76" s="10"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -3786,7 +4251,7 @@
       <c r="S77" s="10"/>
       <c r="T77" s="10"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -3808,7 +4273,7 @@
       <c r="S78" s="10"/>
       <c r="T78" s="10"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -3830,7 +4295,7 @@
       <c r="S79" s="10"/>
       <c r="T79" s="10"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -3852,7 +4317,7 @@
       <c r="S80" s="10"/>
       <c r="T80" s="10"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -3874,7 +4339,7 @@
       <c r="S81" s="10"/>
       <c r="T81" s="10"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -3896,7 +4361,7 @@
       <c r="S82" s="10"/>
       <c r="T82" s="10"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -3918,7 +4383,7 @@
       <c r="S83" s="10"/>
       <c r="T83" s="10"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -3940,7 +4405,7 @@
       <c r="S84" s="10"/>
       <c r="T84" s="10"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -3962,7 +4427,7 @@
       <c r="S85" s="10"/>
       <c r="T85" s="10"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -3984,7 +4449,7 @@
       <c r="S86" s="10"/>
       <c r="T86" s="10"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -4006,7 +4471,7 @@
       <c r="S87" s="10"/>
       <c r="T87" s="10"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -4028,7 +4493,7 @@
       <c r="S88" s="10"/>
       <c r="T88" s="10"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -4050,7 +4515,7 @@
       <c r="S89" s="10"/>
       <c r="T89" s="10"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -4072,7 +4537,7 @@
       <c r="S90" s="10"/>
       <c r="T90" s="10"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -4096,12 +4561,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L58:P58"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="L17:P19"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="L30:P30"/>
-    <mergeCell ref="G17:K22"/>
+    <mergeCell ref="A4:R7"/>
+    <mergeCell ref="L41:P41"/>
+    <mergeCell ref="L38:P40"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="Q42:Q50"/>
+    <mergeCell ref="A42:A50"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="Q53:Q57"/>
     <mergeCell ref="J8:M9"/>
@@ -4118,12 +4583,1939 @@
     <mergeCell ref="B38:F40"/>
     <mergeCell ref="G38:K40"/>
     <mergeCell ref="G51:K51"/>
-    <mergeCell ref="A4:R7"/>
-    <mergeCell ref="L41:P41"/>
-    <mergeCell ref="L38:P40"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="Q42:Q50"/>
-    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="L58:P58"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="L17:P19"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="L30:P30"/>
+    <mergeCell ref="G17:K22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F11287C-6B85-44DE-A4AF-43D9C6758D76}">
+  <dimension ref="A1:T74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="35.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="150">
+        <v>43771</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="199" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="190"/>
+      <c r="N3" s="190"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="200" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="201" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="197" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+    </row>
+    <row r="5" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="202" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="203">
+        <v>65</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+    </row>
+    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="204" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="203">
+        <v>4</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="152" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="153"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="204" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="203">
+        <v>40</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="182" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="13">
+        <v>32</v>
+      </c>
+      <c r="F7" s="13">
+        <v>35</v>
+      </c>
+      <c r="G7" s="13">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13">
+        <v>5</v>
+      </c>
+      <c r="I7" s="13">
+        <v>40</v>
+      </c>
+      <c r="J7" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="187"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="204" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="203">
+        <v>25</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="183" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="119" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="121"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="204" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="203">
+        <f>B5*B6</f>
+        <v>260</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="204" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="203">
+        <f>9*4</f>
+        <v>36</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="155"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="204" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="203">
+        <f t="shared" ref="B11" si="0">B9-B10</f>
+        <v>224</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="182" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="13">
+        <v>32</v>
+      </c>
+      <c r="F11" s="13">
+        <v>35</v>
+      </c>
+      <c r="G11" s="13">
+        <v>8</v>
+      </c>
+      <c r="H11" s="13">
+        <v>5</v>
+      </c>
+      <c r="I11" s="13">
+        <v>40</v>
+      </c>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="204" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="203">
+        <f>B11/40</f>
+        <v>5.6</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="184" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="181" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="188"/>
+      <c r="L12" s="191"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="46">
+        <v>43181</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="178" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="179"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="194"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="17">
+        <v>32</v>
+      </c>
+      <c r="F15" s="18">
+        <v>35</v>
+      </c>
+      <c r="G15" s="18">
+        <v>8</v>
+      </c>
+      <c r="H15" s="18">
+        <v>5</v>
+      </c>
+      <c r="I15" s="173">
+        <v>40</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="192" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="174" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="193" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="176" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="177" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+    </row>
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="209"/>
+      <c r="H19" s="214" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="215"/>
+      <c r="J19" s="215"/>
+      <c r="K19" s="215"/>
+      <c r="L19" s="216"/>
+      <c r="M19" s="189"/>
+      <c r="N19" s="189"/>
+      <c r="O19" s="189"/>
+      <c r="P19" s="189"/>
+      <c r="Q19" s="189"/>
+    </row>
+    <row r="20" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="91"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="210"/>
+      <c r="H20" s="167"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="104"/>
+      <c r="L20" s="217"/>
+      <c r="M20" s="168"/>
+      <c r="N20" s="168"/>
+      <c r="O20" s="168"/>
+      <c r="P20" s="168"/>
+      <c r="Q20" s="168"/>
+    </row>
+    <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="91"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="210"/>
+      <c r="H21" s="167"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="217"/>
+      <c r="M21" s="168"/>
+      <c r="N21" s="168"/>
+      <c r="O21" s="168"/>
+      <c r="P21" s="168"/>
+      <c r="Q21" s="168"/>
+    </row>
+    <row r="22" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="166"/>
+      <c r="B22" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="210"/>
+      <c r="H22" s="167"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="217"/>
+      <c r="M22" s="191"/>
+      <c r="N22" s="191"/>
+      <c r="O22" s="191"/>
+      <c r="P22" s="191"/>
+      <c r="Q22" s="191"/>
+    </row>
+    <row r="23" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="205">
+        <v>42917</v>
+      </c>
+      <c r="B23" s="17">
+        <v>32</v>
+      </c>
+      <c r="C23" s="18">
+        <v>35</v>
+      </c>
+      <c r="D23" s="18">
+        <v>8</v>
+      </c>
+      <c r="E23" s="18">
+        <v>5</v>
+      </c>
+      <c r="F23" s="12">
+        <v>40</v>
+      </c>
+      <c r="G23" s="211" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="167"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="217"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+    </row>
+    <row r="24" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="206"/>
+      <c r="B24" s="31">
+        <v>11</v>
+      </c>
+      <c r="C24" s="70">
+        <v>11</v>
+      </c>
+      <c r="D24" s="70">
+        <v>11</v>
+      </c>
+      <c r="E24" s="24">
+        <v>11</v>
+      </c>
+      <c r="F24" s="32">
+        <v>11</v>
+      </c>
+      <c r="G24" s="211"/>
+      <c r="H24" s="185"/>
+      <c r="I24" s="186"/>
+      <c r="J24" s="186"/>
+      <c r="K24" s="186"/>
+      <c r="L24" s="218"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+    </row>
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="206"/>
+      <c r="B25" s="31">
+        <v>13</v>
+      </c>
+      <c r="C25" s="24">
+        <v>13</v>
+      </c>
+      <c r="D25" s="24">
+        <v>13</v>
+      </c>
+      <c r="E25" s="24">
+        <v>13</v>
+      </c>
+      <c r="F25" s="32">
+        <v>13</v>
+      </c>
+      <c r="G25" s="211"/>
+      <c r="H25" s="219" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="93"/>
+      <c r="J25" s="93"/>
+      <c r="K25" s="93"/>
+      <c r="L25" s="220"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+    </row>
+    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="206"/>
+      <c r="B26" s="31">
+        <v>15</v>
+      </c>
+      <c r="C26" s="24">
+        <v>15</v>
+      </c>
+      <c r="D26" s="24">
+        <v>15</v>
+      </c>
+      <c r="E26" s="24">
+        <v>15</v>
+      </c>
+      <c r="F26" s="32">
+        <v>15</v>
+      </c>
+      <c r="G26" s="211"/>
+      <c r="H26" s="231"/>
+      <c r="I26" s="96"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="232"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+    </row>
+    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="206"/>
+      <c r="B27" s="72">
+        <v>17</v>
+      </c>
+      <c r="C27" s="24">
+        <v>17</v>
+      </c>
+      <c r="D27" s="24">
+        <v>17</v>
+      </c>
+      <c r="E27" s="24">
+        <v>17</v>
+      </c>
+      <c r="F27" s="32">
+        <v>17</v>
+      </c>
+      <c r="G27" s="211"/>
+      <c r="H27" s="233"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="234"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="206"/>
+      <c r="B28" s="31">
+        <v>19</v>
+      </c>
+      <c r="C28" s="24">
+        <v>19</v>
+      </c>
+      <c r="D28" s="24">
+        <v>19</v>
+      </c>
+      <c r="E28" s="24">
+        <v>19</v>
+      </c>
+      <c r="F28" s="32">
+        <v>19</v>
+      </c>
+      <c r="G28" s="211"/>
+      <c r="H28" s="195" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="196"/>
+      <c r="J28" s="196"/>
+      <c r="K28" s="196"/>
+      <c r="L28" s="221"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="206"/>
+      <c r="B29" s="31">
+        <v>21</v>
+      </c>
+      <c r="C29" s="24">
+        <v>21</v>
+      </c>
+      <c r="D29" s="24">
+        <v>21</v>
+      </c>
+      <c r="E29" s="24">
+        <v>21</v>
+      </c>
+      <c r="F29" s="32">
+        <v>21</v>
+      </c>
+      <c r="G29" s="211"/>
+      <c r="H29" s="222">
+        <v>32</v>
+      </c>
+      <c r="I29" s="18">
+        <v>35</v>
+      </c>
+      <c r="J29" s="18">
+        <v>8</v>
+      </c>
+      <c r="K29" s="18">
+        <v>5</v>
+      </c>
+      <c r="L29" s="173">
+        <v>40</v>
+      </c>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="206"/>
+      <c r="B30" s="31">
+        <v>23</v>
+      </c>
+      <c r="C30" s="70">
+        <v>23</v>
+      </c>
+      <c r="D30" s="70">
+        <v>23</v>
+      </c>
+      <c r="E30" s="24">
+        <v>23</v>
+      </c>
+      <c r="F30" s="32">
+        <v>23</v>
+      </c>
+      <c r="G30" s="211"/>
+      <c r="H30" s="223">
+        <v>12</v>
+      </c>
+      <c r="I30" s="31">
+        <v>12</v>
+      </c>
+      <c r="J30" s="31">
+        <v>12</v>
+      </c>
+      <c r="K30" s="31">
+        <v>12</v>
+      </c>
+      <c r="L30" s="224">
+        <v>12</v>
+      </c>
+      <c r="M30" s="191"/>
+      <c r="N30" s="191"/>
+      <c r="O30" s="191"/>
+      <c r="P30" s="191"/>
+      <c r="Q30" s="35"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="207"/>
+      <c r="B31" s="72">
+        <v>25</v>
+      </c>
+      <c r="C31" s="24">
+        <v>25</v>
+      </c>
+      <c r="D31" s="24">
+        <v>25</v>
+      </c>
+      <c r="E31" s="24">
+        <v>25</v>
+      </c>
+      <c r="F31" s="32">
+        <v>25</v>
+      </c>
+      <c r="G31" s="211"/>
+      <c r="H31" s="225">
+        <v>14</v>
+      </c>
+      <c r="I31" s="31">
+        <v>14</v>
+      </c>
+      <c r="J31" s="31">
+        <v>14</v>
+      </c>
+      <c r="K31" s="31">
+        <v>14</v>
+      </c>
+      <c r="L31" s="224">
+        <v>14</v>
+      </c>
+      <c r="M31" s="169"/>
+      <c r="N31" s="169"/>
+      <c r="O31" s="169"/>
+      <c r="P31" s="169"/>
+      <c r="Q31" s="170"/>
+      <c r="T31" s="151"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="205">
+        <v>43252</v>
+      </c>
+      <c r="B32" s="163" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="165"/>
+      <c r="G32" s="212"/>
+      <c r="H32" s="223">
+        <v>16</v>
+      </c>
+      <c r="I32" s="31">
+        <v>16</v>
+      </c>
+      <c r="J32" s="31">
+        <v>16</v>
+      </c>
+      <c r="K32" s="31">
+        <v>16</v>
+      </c>
+      <c r="L32" s="228">
+        <v>16</v>
+      </c>
+      <c r="M32" s="191"/>
+      <c r="N32" s="191"/>
+      <c r="O32" s="191"/>
+      <c r="P32" s="191"/>
+      <c r="Q32" s="191"/>
+      <c r="T32" s="151"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="206"/>
+      <c r="B33" s="17">
+        <v>32</v>
+      </c>
+      <c r="C33" s="18">
+        <v>35</v>
+      </c>
+      <c r="D33" s="18">
+        <v>8</v>
+      </c>
+      <c r="E33" s="18">
+        <v>5</v>
+      </c>
+      <c r="F33" s="12">
+        <v>40</v>
+      </c>
+      <c r="G33" s="210"/>
+      <c r="H33" s="225">
+        <v>18</v>
+      </c>
+      <c r="I33" s="24">
+        <v>18</v>
+      </c>
+      <c r="J33" s="24">
+        <v>18</v>
+      </c>
+      <c r="K33" s="24">
+        <v>18</v>
+      </c>
+      <c r="L33" s="50">
+        <v>18</v>
+      </c>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="T33" s="151"/>
+    </row>
+    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="206"/>
+      <c r="B34" s="31">
+        <v>18</v>
+      </c>
+      <c r="C34" s="70">
+        <v>18</v>
+      </c>
+      <c r="D34" s="24">
+        <v>18</v>
+      </c>
+      <c r="E34" s="24">
+        <v>18</v>
+      </c>
+      <c r="F34" s="73">
+        <v>18</v>
+      </c>
+      <c r="G34" s="211" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="223">
+        <v>20</v>
+      </c>
+      <c r="I34" s="31">
+        <v>20</v>
+      </c>
+      <c r="J34" s="31">
+        <v>20</v>
+      </c>
+      <c r="K34" s="72">
+        <v>20</v>
+      </c>
+      <c r="L34" s="229">
+        <v>20</v>
+      </c>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="T34" s="151"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="206"/>
+      <c r="B35" s="31">
+        <v>20</v>
+      </c>
+      <c r="C35" s="24">
+        <v>20</v>
+      </c>
+      <c r="D35" s="24">
+        <v>20</v>
+      </c>
+      <c r="E35" s="24">
+        <v>20</v>
+      </c>
+      <c r="F35" s="32">
+        <v>20</v>
+      </c>
+      <c r="G35" s="211"/>
+      <c r="H35" s="223">
+        <v>22</v>
+      </c>
+      <c r="I35" s="31">
+        <v>22</v>
+      </c>
+      <c r="J35" s="31">
+        <v>22</v>
+      </c>
+      <c r="K35" s="31">
+        <v>22</v>
+      </c>
+      <c r="L35" s="229">
+        <v>22</v>
+      </c>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="T35" s="151"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="206"/>
+      <c r="B36" s="156">
+        <v>22</v>
+      </c>
+      <c r="C36" s="157">
+        <v>22</v>
+      </c>
+      <c r="D36" s="157">
+        <v>22</v>
+      </c>
+      <c r="E36" s="157">
+        <v>22</v>
+      </c>
+      <c r="F36" s="158">
+        <v>22</v>
+      </c>
+      <c r="G36" s="211"/>
+      <c r="H36" s="226">
+        <v>24</v>
+      </c>
+      <c r="I36" s="156">
+        <v>24</v>
+      </c>
+      <c r="J36" s="159">
+        <v>24</v>
+      </c>
+      <c r="K36" s="159">
+        <v>24</v>
+      </c>
+      <c r="L36" s="224">
+        <v>24</v>
+      </c>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="T36" s="151"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="206"/>
+      <c r="B37" s="159">
+        <v>24</v>
+      </c>
+      <c r="C37" s="157">
+        <v>24</v>
+      </c>
+      <c r="D37" s="157">
+        <v>24</v>
+      </c>
+      <c r="E37" s="157">
+        <v>24</v>
+      </c>
+      <c r="F37" s="158">
+        <v>24</v>
+      </c>
+      <c r="G37" s="211"/>
+      <c r="H37" s="235" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="236"/>
+      <c r="J37" s="236"/>
+      <c r="K37" s="236"/>
+      <c r="L37" s="237"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="T37" s="151"/>
+    </row>
+    <row r="38" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="207"/>
+      <c r="B38" s="160">
+        <v>26</v>
+      </c>
+      <c r="C38" s="161">
+        <v>26</v>
+      </c>
+      <c r="D38" s="161">
+        <v>26</v>
+      </c>
+      <c r="E38" s="161">
+        <v>26</v>
+      </c>
+      <c r="F38" s="162">
+        <v>26</v>
+      </c>
+      <c r="G38" s="213"/>
+      <c r="H38" s="195" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="196"/>
+      <c r="J38" s="196"/>
+      <c r="K38" s="196"/>
+      <c r="L38" s="221"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="T38" s="151"/>
+    </row>
+    <row r="39" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="175"/>
+      <c r="B39" s="208" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="208"/>
+      <c r="D39" s="208"/>
+      <c r="E39" s="208"/>
+      <c r="F39" s="208"/>
+      <c r="G39" s="171"/>
+      <c r="H39" s="222">
+        <v>32</v>
+      </c>
+      <c r="I39" s="18">
+        <v>35</v>
+      </c>
+      <c r="J39" s="18">
+        <v>8</v>
+      </c>
+      <c r="K39" s="18">
+        <v>5</v>
+      </c>
+      <c r="L39" s="173">
+        <v>40</v>
+      </c>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+    </row>
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="225">
+        <v>19</v>
+      </c>
+      <c r="I40" s="24">
+        <v>19</v>
+      </c>
+      <c r="J40" s="24">
+        <v>19</v>
+      </c>
+      <c r="K40" s="70">
+        <v>19</v>
+      </c>
+      <c r="L40" s="50">
+        <v>19</v>
+      </c>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+    </row>
+    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="238" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="239"/>
+      <c r="C41" s="239"/>
+      <c r="D41" s="239"/>
+      <c r="E41" s="239"/>
+      <c r="F41" s="240"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="223">
+        <v>21</v>
+      </c>
+      <c r="I41" s="24">
+        <v>21</v>
+      </c>
+      <c r="J41" s="70">
+        <v>21</v>
+      </c>
+      <c r="K41" s="24">
+        <v>21</v>
+      </c>
+      <c r="L41" s="230">
+        <v>21</v>
+      </c>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+    </row>
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="172"/>
+      <c r="B42" s="241" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="242"/>
+      <c r="F42" s="243"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="223">
+        <v>23</v>
+      </c>
+      <c r="I42" s="24">
+        <v>23</v>
+      </c>
+      <c r="J42" s="24">
+        <v>23</v>
+      </c>
+      <c r="K42" s="70">
+        <v>23</v>
+      </c>
+      <c r="L42" s="50">
+        <v>23</v>
+      </c>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+    </row>
+    <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="172"/>
+      <c r="B43" s="17">
+        <v>32</v>
+      </c>
+      <c r="C43" s="18">
+        <v>35</v>
+      </c>
+      <c r="D43" s="18">
+        <v>8</v>
+      </c>
+      <c r="E43" s="18">
+        <v>5</v>
+      </c>
+      <c r="F43" s="173">
+        <v>40</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="223">
+        <v>25</v>
+      </c>
+      <c r="I43" s="24">
+        <v>25</v>
+      </c>
+      <c r="J43" s="24">
+        <v>25</v>
+      </c>
+      <c r="K43" s="24">
+        <v>25</v>
+      </c>
+      <c r="L43" s="50">
+        <v>25</v>
+      </c>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+    </row>
+    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="193" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="244" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="245" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="245" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="245" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="246" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="227">
+        <v>27</v>
+      </c>
+      <c r="I44" s="25">
+        <v>27</v>
+      </c>
+      <c r="J44" s="25">
+        <v>27</v>
+      </c>
+      <c r="K44" s="25">
+        <v>27</v>
+      </c>
+      <c r="L44" s="54">
+        <v>27</v>
+      </c>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
+      <c r="N62" s="10"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+      <c r="N64" s="10"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="H25:L27"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="H19:L24"/>
+    <mergeCell ref="G23:G31"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H5:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="G34:G38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>